<commit_message>
Finished Diagnosis Classification functionality
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/RuleSets.xlsx
+++ b/Development/Data/MetaData/RuleSets.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B57F686-CED9-4095-9411-0717A48B0326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BFFAA4-1A8F-4634-8D80-A3E136F3F074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="DiagnosisAssociation" sheetId="16" r:id="rId1"/>
-    <sheet name="DiagnosisDuplicates" sheetId="20" r:id="rId2"/>
+    <sheet name="DiagnosisRedundancies" sheetId="20" r:id="rId2"/>
     <sheet name="ExcludeRawData" sheetId="18" r:id="rId3"/>
     <sheet name="TempBackup" sheetId="19" r:id="rId4"/>
   </sheets>
@@ -222,10 +222,10 @@
     <t>InitialDiagnosisDate</t>
   </si>
   <si>
-    <t>IsLikelyDuplicate</t>
-  </si>
-  <si>
     <t>CountDeviatingValues</t>
+  </si>
+  <si>
+    <t>IsLikelyRedundant</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -365,6 +365,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -374,392 +380,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="94">
     <dxf>
       <font>
         <b/>
@@ -2216,49 +1841,32 @@
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="11.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" style="9" customWidth="1"/>
     <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="13" max="15" width="11.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" style="9" customWidth="1"/>
     <col min="17" max="17" width="12.109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="16" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" style="1" customWidth="1"/>
+    <col min="18" max="20" width="11.33203125" style="1" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" style="9" customWidth="1"/>
     <col min="22" max="22" width="12.109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="16" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
+    <col min="23" max="25" width="11.33203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="11.33203125" style="9" customWidth="1"/>
     <col min="27" max="27" width="12.109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.33203125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" style="16" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="1" customWidth="1"/>
+    <col min="28" max="30" width="11.33203125" style="1" customWidth="1"/>
     <col min="31" max="31" width="11.33203125" style="9" customWidth="1"/>
     <col min="32" max="32" width="12.109375" style="1" customWidth="1"/>
     <col min="33" max="33" width="21.88671875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="11.33203125" style="16" customWidth="1"/>
-    <col min="35" max="35" width="11.33203125" style="1" customWidth="1"/>
+    <col min="34" max="35" width="11.33203125" style="1" customWidth="1"/>
     <col min="36" max="36" width="21.33203125" style="9" customWidth="1"/>
     <col min="37" max="37" width="12.109375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.33203125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="11.33203125" style="16" customWidth="1"/>
-    <col min="40" max="40" width="11.33203125" style="1" customWidth="1"/>
+    <col min="38" max="40" width="11.33203125" style="1" customWidth="1"/>
     <col min="41" max="41" width="11.33203125" style="9" customWidth="1"/>
     <col min="42" max="42" width="12.109375" style="1" customWidth="1"/>
-    <col min="43" max="43" width="11.33203125" style="1" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" style="16" customWidth="1"/>
-    <col min="45" max="45" width="11.33203125" style="1" customWidth="1"/>
+    <col min="43" max="45" width="11.33203125" style="1" customWidth="1"/>
     <col min="46" max="46" width="11.33203125" style="9" customWidth="1"/>
     <col min="47" max="47" width="12.109375" style="1" customWidth="1"/>
-    <col min="48" max="48" width="11.33203125" style="1" customWidth="1"/>
-    <col min="49" max="49" width="11.33203125" style="16" customWidth="1"/>
-    <col min="50" max="50" width="11.33203125" style="1" customWidth="1"/>
+    <col min="48" max="50" width="11.33203125" style="1" customWidth="1"/>
     <col min="51" max="51" width="11.33203125" style="9" customWidth="1"/>
     <col min="52" max="52" width="20.109375" style="1" customWidth="1"/>
     <col min="53" max="56" width="27.5546875" style="1" customWidth="1"/>
@@ -2272,69 +1880,69 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="10" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="10" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="10" t="s">
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="10" t="s">
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="10" t="s">
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="10" t="s">
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="10" t="s">
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="12"/>
+      <c r="AV1" s="13"/>
+      <c r="AW1" s="13"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="14"/>
       <c r="AZ1" s="8" t="s">
         <v>14</v>
       </c>
@@ -2364,7 +1972,7 @@
       <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -2379,7 +1987,7 @@
       <c r="M2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -2394,7 +2002,7 @@
       <c r="R2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="3" t="s">
@@ -2409,7 +2017,7 @@
       <c r="W2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="Y2" s="3" t="s">
@@ -2424,7 +2032,7 @@
       <c r="AB2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AD2" s="3" t="s">
@@ -2439,7 +2047,7 @@
       <c r="AG2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AH2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AI2" s="3" t="s">
@@ -2454,7 +2062,7 @@
       <c r="AL2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AN2" s="3" t="s">
@@ -2469,7 +2077,7 @@
       <c r="AQ2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AR2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AS2" s="3" t="s">
@@ -2484,7 +2092,7 @@
       <c r="AV2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="AW2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AX2" s="3" t="s">
@@ -2536,7 +2144,7 @@
         <f>G1&amp;"_"&amp;H2</f>
         <v>ICD10Code_Ref_expr</v>
       </c>
-      <c r="I3" s="15" t="str">
+      <c r="I3" s="6" t="str">
         <f>G1&amp;"_"&amp;I2</f>
         <v>ICD10Code_Conn</v>
       </c>
@@ -2556,7 +2164,7 @@
         <f>L1&amp;"_"&amp;M2</f>
         <v>ICD10CodeShort_Ref_expr</v>
       </c>
-      <c r="N3" s="15" t="str">
+      <c r="N3" s="6" t="str">
         <f>L1&amp;"_"&amp;N2</f>
         <v>ICD10CodeShort_Conn</v>
       </c>
@@ -2576,7 +2184,7 @@
         <f>Q1&amp;"_"&amp;R2</f>
         <v>ICD10Group_Ref_expr</v>
       </c>
-      <c r="S3" s="15" t="str">
+      <c r="S3" s="6" t="str">
         <f>Q1&amp;"_"&amp;S2</f>
         <v>ICD10Group_Conn</v>
       </c>
@@ -2596,7 +2204,7 @@
         <f>V1&amp;"_"&amp;W2</f>
         <v>ICDOTopographyCode_Ref_expr</v>
       </c>
-      <c r="X3" s="15" t="str">
+      <c r="X3" s="6" t="str">
         <f>V1&amp;"_"&amp;X2</f>
         <v>ICDOTopographyCode_Conn</v>
       </c>
@@ -2616,7 +2224,7 @@
         <f>AA1&amp;"_"&amp;AB2</f>
         <v>ICDOTopographyCodeShort_Ref_expr</v>
       </c>
-      <c r="AC3" s="15" t="str">
+      <c r="AC3" s="6" t="str">
         <f>AA1&amp;"_"&amp;AC2</f>
         <v>ICDOTopographyCodeShort_Conn</v>
       </c>
@@ -2636,7 +2244,7 @@
         <f>AF1&amp;"_"&amp;AG2</f>
         <v>LocalizationSide_Ref_expr</v>
       </c>
-      <c r="AH3" s="15" t="str">
+      <c r="AH3" s="6" t="str">
         <f>AF1&amp;"_"&amp;AH2</f>
         <v>LocalizationSide_Conn</v>
       </c>
@@ -2656,7 +2264,7 @@
         <f>AK1&amp;"_"&amp;AL2</f>
         <v>ICDOMorphologyCode_Ref_expr</v>
       </c>
-      <c r="AM3" s="15" t="str">
+      <c r="AM3" s="6" t="str">
         <f>AK1&amp;"_"&amp;AM2</f>
         <v>ICDOMorphologyCode_Conn</v>
       </c>
@@ -2676,7 +2284,7 @@
         <f>AP1&amp;"_"&amp;AQ2</f>
         <v>ICDOMorphologyCodeShort_Ref_expr</v>
       </c>
-      <c r="AR3" s="15" t="str">
+      <c r="AR3" s="6" t="str">
         <f>AP1&amp;"_"&amp;AR2</f>
         <v>ICDOMorphologyCodeShort_Conn</v>
       </c>
@@ -2696,7 +2304,7 @@
         <f>AU1&amp;"_"&amp;AV2</f>
         <v>Grading_Ref_expr</v>
       </c>
-      <c r="AW3" s="15" t="str">
+      <c r="AW3" s="6" t="str">
         <f>AU1&amp;"_"&amp;AW2</f>
         <v>Grading_Conn</v>
       </c>
@@ -2708,23 +2316,23 @@
         <f>AU1&amp;"_"&amp;AY2</f>
         <v>Grading_Cand_expr</v>
       </c>
-      <c r="AZ3" s="15" t="str">
+      <c r="AZ3" s="6" t="str">
         <f t="shared" ref="AZ3:BD3" si="0">AZ1&amp;"_"&amp;AZ2</f>
         <v>Relation_ICD10_expr</v>
       </c>
-      <c r="BA3" s="15" t="str">
+      <c r="BA3" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Relation_ICDOTopography_expr</v>
       </c>
-      <c r="BB3" s="15" t="str">
+      <c r="BB3" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Relation_LocalizationSide_expr</v>
       </c>
-      <c r="BC3" s="15" t="str">
+      <c r="BC3" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Relation_ICDOMorphology_expr</v>
       </c>
-      <c r="BD3" s="15" t="str">
+      <c r="BD3" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Relation_Grading_expr</v>
       </c>
@@ -2745,7 +2353,7 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="16" t="str">
+      <c r="N4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2766,7 +2374,7 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="16" t="str">
+      <c r="S5" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2787,7 +2395,7 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X6" s="16" t="str">
+      <c r="X6" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2808,7 +2416,7 @@
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AC7" s="16" t="str">
+      <c r="AC7" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2833,7 +2441,7 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="16" t="str">
+      <c r="I8" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2858,11 +2466,11 @@
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="16" t="str">
+      <c r="I9" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="N9" s="16" t="str">
+      <c r="N9" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2887,11 +2495,11 @@
       <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="16" t="str">
+      <c r="N10" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="S10" s="16" t="str">
+      <c r="S10" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2916,7 +2524,7 @@
       <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S11" s="16" t="str">
+      <c r="S11" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -2941,7 +2549,7 @@
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X12" s="16" t="str">
+      <c r="X12" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2966,11 +2574,11 @@
       <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X13" s="16" t="str">
+      <c r="X13" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="AC13" s="16" t="str">
+      <c r="AC13" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -2995,7 +2603,7 @@
       <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AC14" s="16" t="str">
+      <c r="AC14" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -3017,7 +2625,7 @@
       <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AH15" s="16" t="s">
+      <c r="AH15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3041,7 +2649,7 @@
       <c r="AG16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AH16" s="16" t="s">
+      <c r="AH16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ16" s="9" t="s">
@@ -3068,7 +2676,7 @@
       <c r="AG17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AH17" s="16" t="s">
+      <c r="AH17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ17" s="9" t="s">
@@ -3095,7 +2703,7 @@
       <c r="AG18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AH18" s="16" t="s">
+      <c r="AH18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ18" s="9" t="s">
@@ -3122,7 +2730,7 @@
       <c r="AG19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AH19" s="16" t="s">
+      <c r="AH19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ19" s="9" t="s">
@@ -3146,7 +2754,7 @@
       <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AH20" s="16" t="str">
+      <c r="AH20" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -3168,7 +2776,7 @@
       <c r="F21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AM21" s="16" t="str">
+      <c r="AM21" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -3180,7 +2788,7 @@
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="13" t="str">
+      <c r="C22" s="10" t="str">
         <f>"'Same entity'"</f>
         <v>'Same entity'</v>
       </c>
@@ -3190,11 +2798,11 @@
       <c r="F22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AM22" s="16" t="str">
+      <c r="AM22" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="AR22" s="16" t="str">
+      <c r="AR22" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -3216,7 +2824,7 @@
       <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AR23" s="16" t="str">
+      <c r="AR23" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -3238,7 +2846,7 @@
       <c r="F24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AW24" s="16" t="str">
+      <c r="AW24" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -3260,7 +2868,7 @@
       <c r="F25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AW25" s="16" t="str">
+      <c r="AW25" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -3286,7 +2894,7 @@
         <f>"== 'Unknown'"</f>
         <v>== 'Unknown'</v>
       </c>
-      <c r="AH26" s="16" t="s">
+      <c r="AH26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ26" s="9" t="str">
@@ -3310,19 +2918,19 @@
       <c r="F27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="16" t="str">
+      <c r="I27" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="X27" s="16" t="str">
+      <c r="X27" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="AM27" s="16" t="str">
+      <c r="AM27" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="AR27" s="17"/>
+      <c r="AR27" s="10"/>
     </row>
     <row r="28" spans="1:51" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
@@ -3344,7 +2952,7 @@
         <f>"== 'Low grade'"</f>
         <v>== 'Low grade'</v>
       </c>
-      <c r="AW28" s="16" t="s">
+      <c r="AW28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AY28" s="9" t="str">
@@ -3373,7 +2981,7 @@
         <f>"%in% c('Left', 'Right', 'Midline', 'Bilateral')"</f>
         <v>%in% c('Left', 'Right', 'Midline', 'Bilateral')</v>
       </c>
-      <c r="AH29" s="16" t="s">
+      <c r="AH29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ29" s="9" t="str">
@@ -3402,7 +3010,7 @@
         <f>"== 'Inapplicable'"</f>
         <v>== 'Inapplicable'</v>
       </c>
-      <c r="AH30" s="16" t="s">
+      <c r="AH30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AJ30" s="9" t="str">
@@ -3424,47 +3032,47 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G4:BD995">
-    <cfRule type="expression" dxfId="123" priority="109">
+    <cfRule type="expression" dxfId="93" priority="109">
       <formula>NOT(ISBLANK(G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I188">
-    <cfRule type="expression" dxfId="122" priority="108">
+    <cfRule type="expression" dxfId="92" priority="108">
       <formula>NOT(ISBLANK(I4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N188">
-    <cfRule type="expression" dxfId="121" priority="107">
+    <cfRule type="expression" dxfId="91" priority="107">
       <formula>NOT(ISBLANK(N4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S188">
-    <cfRule type="expression" dxfId="120" priority="106">
+    <cfRule type="expression" dxfId="90" priority="106">
       <formula>NOT(ISBLANK(S4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X4:X188">
-    <cfRule type="expression" dxfId="119" priority="105">
+    <cfRule type="expression" dxfId="89" priority="105">
       <formula>NOT(ISBLANK(X4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC188">
-    <cfRule type="expression" dxfId="118" priority="104">
+    <cfRule type="expression" dxfId="88" priority="104">
       <formula>NOT(ISBLANK(AC4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4:AH188">
-    <cfRule type="expression" dxfId="117" priority="103">
+    <cfRule type="expression" dxfId="87" priority="103">
       <formula>NOT(ISBLANK(AH4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR4:AR188">
-    <cfRule type="expression" dxfId="116" priority="101">
+    <cfRule type="expression" dxfId="86" priority="101">
       <formula>NOT(ISBLANK(AR4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW4:AW188">
-    <cfRule type="expression" dxfId="115" priority="100">
+    <cfRule type="expression" dxfId="85" priority="100">
       <formula>NOT(ISBLANK(AW4))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3481,7 +3089,7 @@
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3493,43 +3101,27 @@
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="11.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" style="9" customWidth="1"/>
     <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="13" max="15" width="11.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" style="9" customWidth="1"/>
     <col min="17" max="17" width="12.109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="16" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" style="1" customWidth="1"/>
+    <col min="18" max="20" width="11.33203125" style="1" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" style="9" customWidth="1"/>
     <col min="22" max="22" width="12.109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="11.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="11.33203125" style="16" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
+    <col min="23" max="25" width="11.33203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="11.33203125" style="9" customWidth="1"/>
-    <col min="27" max="28" width="12.88671875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.88671875" style="16" customWidth="1"/>
-    <col min="30" max="30" width="12.88671875" style="1" customWidth="1"/>
+    <col min="27" max="30" width="12.88671875" style="1" customWidth="1"/>
     <col min="31" max="31" width="12.88671875" style="9" customWidth="1"/>
     <col min="32" max="32" width="12.109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="11.33203125" style="16" customWidth="1"/>
-    <col min="35" max="35" width="11.33203125" style="1" customWidth="1"/>
+    <col min="33" max="35" width="11.33203125" style="1" customWidth="1"/>
     <col min="36" max="36" width="11.33203125" style="9" customWidth="1"/>
     <col min="37" max="37" width="12.109375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.33203125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="11.33203125" style="16" customWidth="1"/>
-    <col min="40" max="40" width="11.33203125" style="1" customWidth="1"/>
+    <col min="38" max="40" width="11.33203125" style="1" customWidth="1"/>
     <col min="41" max="41" width="11.33203125" style="9" customWidth="1"/>
     <col min="42" max="42" width="12.109375" style="1" customWidth="1"/>
-    <col min="43" max="43" width="11.33203125" style="1" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" style="16" customWidth="1"/>
-    <col min="45" max="45" width="11.33203125" style="1" customWidth="1"/>
+    <col min="43" max="45" width="11.33203125" style="1" customWidth="1"/>
     <col min="46" max="46" width="11.33203125" style="9" customWidth="1"/>
     <col min="47" max="16384" width="16.33203125" style="1"/>
   </cols>
@@ -3541,62 +3133,62 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="G1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="10" t="s">
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="10" t="s">
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="10" t="s">
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="10" t="s">
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="13"/>
+      <c r="AJ1" s="13"/>
+      <c r="AK1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="10" t="s">
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="13"/>
+      <c r="AP1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="12"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="14"/>
     </row>
     <row r="2" spans="1:46" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -3611,7 +3203,7 @@
       <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -3626,7 +3218,7 @@
       <c r="M2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -3641,7 +3233,7 @@
       <c r="R2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="3" t="s">
@@ -3656,7 +3248,7 @@
       <c r="W2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="Y2" s="3" t="s">
@@ -3671,7 +3263,7 @@
       <c r="AB2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AD2" s="3" t="s">
@@ -3686,7 +3278,7 @@
       <c r="AG2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AH2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AI2" s="3" t="s">
@@ -3701,7 +3293,7 @@
       <c r="AL2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AN2" s="3" t="s">
@@ -3716,7 +3308,7 @@
       <c r="AQ2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AR2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AS2" s="3" t="s">
@@ -3753,7 +3345,7 @@
         <f>G1&amp;"_"&amp;H2</f>
         <v>CountDeviatingValues_Ref_expr</v>
       </c>
-      <c r="I3" s="15" t="str">
+      <c r="I3" s="6" t="str">
         <f>G1&amp;"_"&amp;I2</f>
         <v>CountDeviatingValues_Conn</v>
       </c>
@@ -3773,7 +3365,7 @@
         <f>L1&amp;"_"&amp;M2</f>
         <v>InitialDiagnosisDate_Ref_expr</v>
       </c>
-      <c r="N3" s="15" t="str">
+      <c r="N3" s="6" t="str">
         <f>L1&amp;"_"&amp;N2</f>
         <v>InitialDiagnosisDate_Conn</v>
       </c>
@@ -3793,7 +3385,7 @@
         <f>Q1&amp;"_"&amp;R2</f>
         <v>ICD10Code_Ref_expr</v>
       </c>
-      <c r="S3" s="15" t="str">
+      <c r="S3" s="6" t="str">
         <f>Q1&amp;"_"&amp;S2</f>
         <v>ICD10Code_Conn</v>
       </c>
@@ -3813,7 +3405,7 @@
         <f>V1&amp;"_"&amp;W2</f>
         <v>ICDOTopographyCode_Ref_expr</v>
       </c>
-      <c r="X3" s="15" t="str">
+      <c r="X3" s="6" t="str">
         <f>V1&amp;"_"&amp;X2</f>
         <v>ICDOTopographyCode_Conn</v>
       </c>
@@ -3833,7 +3425,7 @@
         <f>AA1&amp;"_"&amp;AB2</f>
         <v>LocalizationSide_Ref_expr</v>
       </c>
-      <c r="AC3" s="15" t="str">
+      <c r="AC3" s="6" t="str">
         <f>AA1&amp;"_"&amp;AC2</f>
         <v>LocalizationSide_Conn</v>
       </c>
@@ -3853,7 +3445,7 @@
         <f>AF1&amp;"_"&amp;AG2</f>
         <v>HistologyDate_Ref_expr</v>
       </c>
-      <c r="AH3" s="15" t="str">
+      <c r="AH3" s="6" t="str">
         <f>AF1&amp;"_"&amp;AH2</f>
         <v>HistologyDate_Conn</v>
       </c>
@@ -3873,7 +3465,7 @@
         <f>AK1&amp;"_"&amp;AL2</f>
         <v>ICDOMorphologyCode_Ref_expr</v>
       </c>
-      <c r="AM3" s="15" t="str">
+      <c r="AM3" s="6" t="str">
         <f>AK1&amp;"_"&amp;AM2</f>
         <v>ICDOMorphologyCode_Conn</v>
       </c>
@@ -3893,7 +3485,7 @@
         <f>AP1&amp;"_"&amp;AQ2</f>
         <v>Grading_Ref_expr</v>
       </c>
-      <c r="AR3" s="15" t="str">
+      <c r="AR3" s="6" t="str">
         <f>AP1&amp;"_"&amp;AR2</f>
         <v>Grading_Conn</v>
       </c>
@@ -3911,7 +3503,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -3922,31 +3514,31 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="16" t="str">
+      <c r="N4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="S4" s="16" t="str">
+      <c r="S4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="X4" s="16" t="str">
+      <c r="X4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="AC4" s="16" t="str">
+      <c r="AC4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="AH4" s="16" t="str">
+      <c r="AH4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="AM4" s="16" t="str">
+      <c r="AM4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="AR4" s="16" t="str">
+      <c r="AR4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -3956,9 +3548,9 @@
         <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -3968,13 +3560,13 @@
         <v>16</v>
       </c>
       <c r="K5" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" ref="K5:K11" si="0">"&lt;= 1"</f>
         <v>&lt;= 1</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -3986,9 +3578,9 @@
         <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1">
@@ -3997,16 +3589,14 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="1"/>
       <c r="K6" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" si="0"/>
         <v>&lt;= 1</v>
       </c>
-      <c r="N6" s="1"/>
       <c r="Q6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="16" t="s">
+      <c r="S6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="T6" s="1" t="s">
@@ -4018,9 +3608,9 @@
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1">
@@ -4030,13 +3620,13 @@
         <v>16</v>
       </c>
       <c r="K7" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" si="0"/>
         <v>&lt;= 1</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X7" s="16" t="s">
+      <c r="X7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="Y7" s="1" t="s">
@@ -4048,9 +3638,9 @@
         <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="1">
@@ -4060,13 +3650,13 @@
         <v>16</v>
       </c>
       <c r="K8" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" si="0"/>
         <v>&lt;= 1</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AC8" s="16" t="s">
+      <c r="AC8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AD8" s="1" t="s">
@@ -4078,9 +3668,9 @@
         <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1">
@@ -4090,29 +3680,27 @@
         <v>16</v>
       </c>
       <c r="K9" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" si="0"/>
         <v>&lt;= 1</v>
       </c>
-      <c r="AC9" s="1"/>
       <c r="AF9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AH9" s="16" t="s">
+      <c r="AH9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AI9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AM9" s="1"/>
     </row>
     <row r="10" spans="1:46" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1">
@@ -4122,15 +3710,13 @@
         <v>16</v>
       </c>
       <c r="K10" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" si="0"/>
         <v>&lt;= 1</v>
       </c>
-      <c r="AC10" s="1"/>
-      <c r="AH10" s="1"/>
       <c r="AK10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AM10" s="16" t="s">
+      <c r="AM10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AN10" s="1" t="s">
@@ -4142,9 +3728,9 @@
         <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1">
@@ -4154,16 +3740,13 @@
         <v>16</v>
       </c>
       <c r="K11" s="9" t="str">
-        <f>"&lt;= 1"</f>
+        <f t="shared" si="0"/>
         <v>&lt;= 1</v>
       </c>
-      <c r="AC11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AM11" s="1"/>
       <c r="AP11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AR11" s="16" t="s">
+      <c r="AR11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="AS11" s="1" t="s">
@@ -4171,7 +3754,7 @@
       </c>
     </row>
     <row r="25" spans="3:3" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="13"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="29" spans="3:3" ht="46.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -4186,412 +3769,412 @@
     <mergeCell ref="AA1:AE1"/>
   </mergeCells>
   <conditionalFormatting sqref="U5:AE5 Q4:AE4 Q6:U6 Z6:AE6 Q7:Z7 AE7 AJ8 AO8:AT8 AK10:AN10 AF9:AT9 L12:AT998 AF4:AT7 Q8:AE9 L4:P9">
-    <cfRule type="expression" dxfId="114" priority="200">
+    <cfRule type="expression" dxfId="84" priority="200">
       <formula>NOT(ISBLANK(L4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X4">
-    <cfRule type="expression" dxfId="113" priority="196">
+    <cfRule type="expression" dxfId="83" priority="196">
       <formula>NOT(ISBLANK(X4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR4:AR5">
-    <cfRule type="expression" dxfId="112" priority="191">
+    <cfRule type="expression" dxfId="82" priority="191">
       <formula>NOT(ISBLANK(AR4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V5:W5 Y5">
-    <cfRule type="expression" dxfId="111" priority="190">
+    <cfRule type="expression" dxfId="81" priority="190">
       <formula>NOT(ISBLANK(V5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X5">
-    <cfRule type="expression" dxfId="110" priority="189">
+    <cfRule type="expression" dxfId="80" priority="189">
       <formula>NOT(ISBLANK(X5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S7">
-    <cfRule type="expression" dxfId="109" priority="188">
+    <cfRule type="expression" dxfId="79" priority="188">
       <formula>NOT(ISBLANK(S7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM7">
-    <cfRule type="expression" dxfId="108" priority="184">
+    <cfRule type="expression" dxfId="78" priority="184">
       <formula>NOT(ISBLANK(AM7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR7">
-    <cfRule type="expression" dxfId="107" priority="182">
+    <cfRule type="expression" dxfId="77" priority="182">
       <formula>NOT(ISBLANK(AR7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK10:AN10">
-    <cfRule type="expression" dxfId="106" priority="179">
+    <cfRule type="expression" dxfId="76" priority="179">
       <formula>NOT(ISBLANK(AK10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8:R8 T8:U8 AE8 AO8 AS8:AT8 Z8">
-    <cfRule type="expression" dxfId="105" priority="178">
+    <cfRule type="expression" dxfId="75" priority="178">
       <formula>NOT(ISBLANK(Q8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8">
-    <cfRule type="expression" dxfId="104" priority="177">
+    <cfRule type="expression" dxfId="74" priority="177">
       <formula>NOT(ISBLANK(S8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR8">
-    <cfRule type="expression" dxfId="103" priority="172">
+    <cfRule type="expression" dxfId="73" priority="172">
       <formula>NOT(ISBLANK(AR8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V8:W8 Y8">
-    <cfRule type="expression" dxfId="102" priority="171">
+    <cfRule type="expression" dxfId="72" priority="171">
       <formula>NOT(ISBLANK(V8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X8">
-    <cfRule type="expression" dxfId="101" priority="170">
+    <cfRule type="expression" dxfId="71" priority="170">
       <formula>NOT(ISBLANK(X8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP9:AS9">
-    <cfRule type="expression" dxfId="100" priority="169">
+    <cfRule type="expression" dxfId="70" priority="169">
       <formula>NOT(ISBLANK(AP9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9:R9 T9:U9 AE9 AO9 AT9 Z9">
-    <cfRule type="expression" dxfId="99" priority="168">
+    <cfRule type="expression" dxfId="69" priority="168">
       <formula>NOT(ISBLANK(Q9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="expression" dxfId="98" priority="167">
+    <cfRule type="expression" dxfId="68" priority="167">
       <formula>NOT(ISBLANK(S9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V9:W9 Y9">
-    <cfRule type="expression" dxfId="97" priority="162">
+    <cfRule type="expression" dxfId="67" priority="162">
       <formula>NOT(ISBLANK(V9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X9">
-    <cfRule type="expression" dxfId="96" priority="161">
+    <cfRule type="expression" dxfId="66" priority="161">
       <formula>NOT(ISBLANK(X9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN6:AO6 AS6:AT6 Z6 AE6 AK6:AL6">
-    <cfRule type="expression" dxfId="95" priority="158">
+    <cfRule type="expression" dxfId="65" priority="158">
       <formula>NOT(ISBLANK(Z6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7">
-    <cfRule type="expression" dxfId="94" priority="157">
+    <cfRule type="expression" dxfId="64" priority="157">
       <formula>NOT(ISBLANK(X7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR6">
-    <cfRule type="expression" dxfId="93" priority="152">
+    <cfRule type="expression" dxfId="63" priority="152">
       <formula>NOT(ISBLANK(AR6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:M8 O8:P8">
-    <cfRule type="expression" dxfId="88" priority="84">
+    <cfRule type="expression" dxfId="62" priority="84">
       <formula>NOT(ISBLANK(L8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8">
-    <cfRule type="expression" dxfId="87" priority="83">
+    <cfRule type="expression" dxfId="61" priority="83">
       <formula>NOT(ISBLANK(N8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH7">
-    <cfRule type="expression" dxfId="86" priority="98">
+    <cfRule type="expression" dxfId="60" priority="98">
       <formula>NOT(ISBLANK(AH7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF9:AI9">
-    <cfRule type="expression" dxfId="85" priority="97">
+    <cfRule type="expression" dxfId="59" priority="97">
       <formula>NOT(ISBLANK(AF9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ8">
-    <cfRule type="expression" dxfId="84" priority="96">
+    <cfRule type="expression" dxfId="58" priority="96">
       <formula>NOT(ISBLANK(AJ8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ9">
-    <cfRule type="expression" dxfId="83" priority="95">
+    <cfRule type="expression" dxfId="57" priority="95">
       <formula>NOT(ISBLANK(AJ9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6:AJ6 AF6:AG6">
-    <cfRule type="expression" dxfId="82" priority="94">
+    <cfRule type="expression" dxfId="56" priority="94">
       <formula>NOT(ISBLANK(AF6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:AE10 AK10:AQ10 AS10:AT10">
-    <cfRule type="expression" dxfId="81" priority="73">
+    <cfRule type="expression" dxfId="55" priority="73">
       <formula>NOT(ISBLANK(Q10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10:R10 T10:U10 AE10 AO10 AT10 Z10">
-    <cfRule type="expression" dxfId="80" priority="71">
+    <cfRule type="expression" dxfId="54" priority="71">
       <formula>NOT(ISBLANK(Q10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N5">
-    <cfRule type="expression" dxfId="79" priority="86">
+    <cfRule type="expression" dxfId="53" priority="86">
       <formula>NOT(ISBLANK(N4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="expression" dxfId="78" priority="85">
+    <cfRule type="expression" dxfId="52" priority="85">
       <formula>NOT(ISBLANK(N7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:M9 O9:P9">
-    <cfRule type="expression" dxfId="75" priority="82">
+    <cfRule type="expression" dxfId="51" priority="82">
       <formula>NOT(ISBLANK(L9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9">
-    <cfRule type="expression" dxfId="74" priority="81">
+    <cfRule type="expression" dxfId="50" priority="81">
       <formula>NOT(ISBLANK(N9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:M10 O10:P10">
-    <cfRule type="expression" dxfId="73" priority="58">
+    <cfRule type="expression" dxfId="49" priority="58">
       <formula>NOT(ISBLANK(L10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="expression" dxfId="72" priority="57">
+    <cfRule type="expression" dxfId="48" priority="57">
       <formula>NOT(ISBLANK(N10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP10:AQ10 AS10">
-    <cfRule type="expression" dxfId="70" priority="72">
+    <cfRule type="expression" dxfId="47" priority="72">
       <formula>NOT(ISBLANK(AP10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10">
-    <cfRule type="expression" dxfId="68" priority="70">
+    <cfRule type="expression" dxfId="46" priority="70">
       <formula>NOT(ISBLANK(S10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10:W10 Y10">
-    <cfRule type="expression" dxfId="67" priority="69">
+    <cfRule type="expression" dxfId="45" priority="69">
       <formula>NOT(ISBLANK(V10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X10">
-    <cfRule type="expression" dxfId="66" priority="68">
+    <cfRule type="expression" dxfId="44" priority="68">
       <formula>NOT(ISBLANK(X10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V11:W11 Y11">
-    <cfRule type="expression" dxfId="65" priority="50">
+    <cfRule type="expression" dxfId="43" priority="50">
       <formula>NOT(ISBLANK(V11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X11">
-    <cfRule type="expression" dxfId="64" priority="49">
+    <cfRule type="expression" dxfId="42" priority="49">
       <formula>NOT(ISBLANK(X11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10:AJ10">
-    <cfRule type="expression" dxfId="60" priority="62">
+    <cfRule type="expression" dxfId="41" priority="62">
       <formula>NOT(ISBLANK(AF10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="expression" dxfId="59" priority="61">
+    <cfRule type="expression" dxfId="40" priority="61">
       <formula>NOT(ISBLANK(AJ10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF11:AJ11">
-    <cfRule type="expression" dxfId="58" priority="43">
+    <cfRule type="expression" dxfId="39" priority="43">
       <formula>NOT(ISBLANK(AF11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10:P10">
-    <cfRule type="expression" dxfId="57" priority="59">
+    <cfRule type="expression" dxfId="38" priority="59">
       <formula>NOT(ISBLANK(L10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:M11 O11:P11">
-    <cfRule type="expression" dxfId="54" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>NOT(ISBLANK(L11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="expression" dxfId="53" priority="38">
+    <cfRule type="expression" dxfId="36" priority="38">
       <formula>NOT(ISBLANK(N11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11:AE11 AK11:AT11">
-    <cfRule type="expression" dxfId="52" priority="54">
+    <cfRule type="expression" dxfId="35" priority="54">
       <formula>NOT(ISBLANK(Q11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP11:AS11">
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="34" priority="53">
       <formula>NOT(ISBLANK(AP11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q11:R11 T11:U11 AE11 AO11 AT11 Z11">
-    <cfRule type="expression" dxfId="50" priority="52">
+    <cfRule type="expression" dxfId="33" priority="52">
       <formula>NOT(ISBLANK(Q11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11">
-    <cfRule type="expression" dxfId="49" priority="51">
+    <cfRule type="expression" dxfId="32" priority="51">
       <formula>NOT(ISBLANK(S11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6">
-    <cfRule type="expression" dxfId="46" priority="31">
+    <cfRule type="expression" dxfId="31" priority="31">
       <formula>NOT(ISBLANK(X6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC7">
-    <cfRule type="expression" dxfId="44" priority="29">
+    <cfRule type="expression" dxfId="30" priority="29">
       <formula>NOT(ISBLANK(AC7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH8">
-    <cfRule type="expression" dxfId="43" priority="28">
+    <cfRule type="expression" dxfId="29" priority="28">
       <formula>NOT(ISBLANK(AH8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH8">
-    <cfRule type="expression" dxfId="42" priority="27">
+    <cfRule type="expression" dxfId="28" priority="27">
       <formula>NOT(ISBLANK(AH8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ11">
-    <cfRule type="expression" dxfId="40" priority="42">
+    <cfRule type="expression" dxfId="27" priority="42">
       <formula>NOT(ISBLANK(AJ11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM8">
-    <cfRule type="expression" dxfId="39" priority="24">
+    <cfRule type="expression" dxfId="26" priority="24">
       <formula>NOT(ISBLANK(AM8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11:P11">
-    <cfRule type="expression" dxfId="38" priority="40">
+    <cfRule type="expression" dxfId="25" priority="40">
       <formula>NOT(ISBLANK(L11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR10">
-    <cfRule type="expression" dxfId="35" priority="20">
+    <cfRule type="expression" dxfId="24" priority="20">
       <formula>NOT(ISBLANK(AR10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR10">
-    <cfRule type="expression" dxfId="34" priority="19">
+    <cfRule type="expression" dxfId="23" priority="19">
       <formula>NOT(ISBLANK(AR10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="22" priority="35">
       <formula>NOT(ISBLANK(S5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="expression" dxfId="32" priority="34">
+    <cfRule type="expression" dxfId="21" priority="34">
       <formula>NOT(ISBLANK(S5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6">
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>NOT(ISBLANK(X6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM8">
-    <cfRule type="expression" dxfId="26" priority="25">
+    <cfRule type="expression" dxfId="19" priority="25">
       <formula>NOT(ISBLANK(AM8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR9">
-    <cfRule type="expression" dxfId="24" priority="22">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>NOT(ISBLANK(AR9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>NOT(ISBLANK(K11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12:K998 G4:K9">
-    <cfRule type="expression" dxfId="19" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>NOT(ISBLANK(G4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I5">
-    <cfRule type="expression" dxfId="18" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>NOT(ISBLANK(I4))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>NOT(ISBLANK(I7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:H8 J8:K8">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>NOT(ISBLANK(G8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>NOT(ISBLANK(I8))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:H9 J9:K9">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>NOT(ISBLANK(G9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>NOT(ISBLANK(I9))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:J10">
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>NOT(ISBLANK(G10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:H10 J10">
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>NOT(ISBLANK(G10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>NOT(ISBLANK(I10))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:J11">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>NOT(ISBLANK(G11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:H11 J11">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>NOT(ISBLANK(G11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>NOT(ISBLANK(I11))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>NOT(ISBLANK(K10))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4642,41 +4225,41 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="10" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="10" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="10" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="10" t="s">
+      <c r="P1" s="13"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="18"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="10" t="s">
+      <c r="S1" s="13"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="18"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="10" t="s">
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="12"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="14"/>
     </row>
     <row r="2" spans="1:26" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -5025,18 +4608,18 @@
       </c>
     </row>
     <row r="24" spans="4:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="13"/>
+      <c r="D24" s="10"/>
     </row>
     <row r="28" spans="4:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="X1:Z1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X1:Z1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:Z7 F10:Z190 L8:Z9">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -5077,58 +4660,33 @@
     <col min="4" max="4" width="12.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" style="16" customWidth="1"/>
+    <col min="7" max="10" width="11.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" style="9" customWidth="1"/>
     <col min="12" max="12" width="12.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="16" customWidth="1"/>
+    <col min="13" max="16" width="11.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="11.33203125" style="9" customWidth="1"/>
     <col min="18" max="18" width="12.109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" style="16" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" style="16" customWidth="1"/>
+    <col min="19" max="22" width="11.33203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="11.33203125" style="9" customWidth="1"/>
     <col min="24" max="24" width="12.109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" style="16" customWidth="1"/>
-    <col min="27" max="27" width="11.33203125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.33203125" style="16" customWidth="1"/>
+    <col min="25" max="28" width="11.33203125" style="1" customWidth="1"/>
     <col min="29" max="29" width="11.33203125" style="9" customWidth="1"/>
     <col min="30" max="30" width="12.109375" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.33203125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="11.33203125" style="16" customWidth="1"/>
-    <col min="33" max="33" width="11.33203125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="11.33203125" style="16" customWidth="1"/>
+    <col min="31" max="34" width="11.33203125" style="1" customWidth="1"/>
     <col min="35" max="35" width="11.33203125" style="9" customWidth="1"/>
     <col min="36" max="36" width="12.109375" style="1" customWidth="1"/>
     <col min="37" max="37" width="21.88671875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="11.33203125" style="16" customWidth="1"/>
-    <col min="39" max="39" width="11.33203125" style="1" customWidth="1"/>
-    <col min="40" max="40" width="21.33203125" style="16" customWidth="1"/>
+    <col min="38" max="39" width="11.33203125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="21.33203125" style="1" customWidth="1"/>
     <col min="41" max="41" width="11.33203125" style="9" customWidth="1"/>
     <col min="42" max="42" width="12.109375" style="1" customWidth="1"/>
-    <col min="43" max="43" width="11.33203125" style="1" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" style="16" customWidth="1"/>
-    <col min="45" max="45" width="11.33203125" style="1" customWidth="1"/>
-    <col min="46" max="46" width="11.33203125" style="16" customWidth="1"/>
+    <col min="43" max="46" width="11.33203125" style="1" customWidth="1"/>
     <col min="47" max="47" width="11.33203125" style="9" customWidth="1"/>
     <col min="48" max="48" width="12.109375" style="1" customWidth="1"/>
-    <col min="49" max="49" width="11.33203125" style="1" customWidth="1"/>
-    <col min="50" max="50" width="11.33203125" style="16" customWidth="1"/>
-    <col min="51" max="51" width="11.33203125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="11.33203125" style="16" customWidth="1"/>
+    <col min="49" max="52" width="11.33203125" style="1" customWidth="1"/>
     <col min="53" max="53" width="11.33203125" style="9" customWidth="1"/>
     <col min="54" max="54" width="12.109375" style="1" customWidth="1"/>
-    <col min="55" max="55" width="11.33203125" style="1" customWidth="1"/>
-    <col min="56" max="56" width="11.33203125" style="16" customWidth="1"/>
-    <col min="57" max="57" width="11.33203125" style="1" customWidth="1"/>
-    <col min="58" max="58" width="11.33203125" style="16" customWidth="1"/>
+    <col min="55" max="58" width="11.33203125" style="1" customWidth="1"/>
     <col min="59" max="59" width="11.33203125" style="9" customWidth="1"/>
     <col min="60" max="60" width="20.109375" style="1" customWidth="1"/>
     <col min="61" max="64" width="27.5546875" style="1" customWidth="1"/>
@@ -5141,78 +4699,78 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="10" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="10" t="s">
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="10" t="s">
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="10" t="s">
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="10" t="s">
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="10" t="s">
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="13"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="10" t="s">
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="10" t="s">
+      <c r="AW1" s="13"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="13"/>
+      <c r="AZ1" s="13"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="18"/>
-      <c r="BF1" s="18"/>
-      <c r="BG1" s="12"/>
+      <c r="BC1" s="13"/>
+      <c r="BD1" s="13"/>
+      <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="14"/>
       <c r="BH1" s="2"/>
       <c r="BI1" s="2"/>
       <c r="BJ1" s="2"/>
@@ -5231,16 +4789,16 @@
       <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -5249,16 +4807,16 @@
       <c r="M2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -5267,16 +4825,16 @@
       <c r="S2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="W2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="X2" s="3" t="s">
@@ -5285,16 +4843,16 @@
       <c r="Y2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="19" t="s">
+      <c r="AC2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AD2" s="3" t="s">
@@ -5303,16 +4861,16 @@
       <c r="AE2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="14" t="s">
+      <c r="AF2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AH2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AI2" s="19" t="s">
+      <c r="AI2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AJ2" s="3" t="s">
@@ -5321,16 +4879,16 @@
       <c r="AK2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AL2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AM2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN2" s="14" t="s">
+      <c r="AN2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AO2" s="19" t="s">
+      <c r="AO2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AP2" s="3" t="s">
@@ -5339,16 +4897,16 @@
       <c r="AQ2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AR2" s="14" t="s">
+      <c r="AR2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AS2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AT2" s="14" t="s">
+      <c r="AT2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AU2" s="19" t="s">
+      <c r="AU2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="AV2" s="3" t="s">
@@ -5357,16 +4915,16 @@
       <c r="AW2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="AX2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AZ2" s="14" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BA2" s="19" t="s">
+      <c r="BA2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="BB2" s="3" t="s">
@@ -5375,16 +4933,16 @@
       <c r="BC2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="BD2" s="14" t="s">
+      <c r="BD2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="BF2" s="14" t="s">
+      <c r="BF2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="BG2" s="19" t="s">
+      <c r="BG2" s="11" t="s">
         <v>57</v>
       </c>
       <c r="BH2" s="2"/>
@@ -5417,7 +4975,7 @@
         <f>F1&amp;"_"&amp;G2</f>
         <v>ICD10Code_Ref_expr</v>
       </c>
-      <c r="H3" s="15" t="str">
+      <c r="H3" s="6" t="str">
         <f>F1&amp;"_"&amp;H2</f>
         <v>ICD10Code_Conn</v>
       </c>
@@ -5425,7 +4983,7 @@
         <f>F1&amp;"_"&amp;I2</f>
         <v>ICD10Code_Cand_f</v>
       </c>
-      <c r="J3" s="15" t="str">
+      <c r="J3" s="6" t="str">
         <f>F1&amp;"_"&amp;J2</f>
         <v>ICD10Code_Cand_expr</v>
       </c>
@@ -5441,7 +4999,7 @@
         <f>L1&amp;"_"&amp;M2</f>
         <v>ICD10CodeShort_Ref_expr</v>
       </c>
-      <c r="N3" s="15" t="str">
+      <c r="N3" s="6" t="str">
         <f>L1&amp;"_"&amp;N2</f>
         <v>ICD10CodeShort_Conn</v>
       </c>
@@ -5449,7 +5007,7 @@
         <f>L1&amp;"_"&amp;O2</f>
         <v>ICD10CodeShort_Cand_f</v>
       </c>
-      <c r="P3" s="15" t="str">
+      <c r="P3" s="6" t="str">
         <f>L1&amp;"_"&amp;P2</f>
         <v>ICD10CodeShort_Cand_expr</v>
       </c>
@@ -5465,7 +5023,7 @@
         <f>R1&amp;"_"&amp;S2</f>
         <v>ICD10Group_Ref_expr</v>
       </c>
-      <c r="T3" s="15" t="str">
+      <c r="T3" s="6" t="str">
         <f>R1&amp;"_"&amp;T2</f>
         <v>ICD10Group_Conn</v>
       </c>
@@ -5473,7 +5031,7 @@
         <f>R1&amp;"_"&amp;U2</f>
         <v>ICD10Group_Cand_f</v>
       </c>
-      <c r="V3" s="15" t="str">
+      <c r="V3" s="6" t="str">
         <f>R1&amp;"_"&amp;V2</f>
         <v>ICD10Group_Cand_expr</v>
       </c>
@@ -5489,7 +5047,7 @@
         <f>X1&amp;"_"&amp;Y2</f>
         <v>ICDOTopographyCode_Ref_expr</v>
       </c>
-      <c r="Z3" s="15" t="str">
+      <c r="Z3" s="6" t="str">
         <f>X1&amp;"_"&amp;Z2</f>
         <v>ICDOTopographyCode_Conn</v>
       </c>
@@ -5497,7 +5055,7 @@
         <f>X1&amp;"_"&amp;AA2</f>
         <v>ICDOTopographyCode_Cand_f</v>
       </c>
-      <c r="AB3" s="15" t="str">
+      <c r="AB3" s="6" t="str">
         <f>X1&amp;"_"&amp;AB2</f>
         <v>ICDOTopographyCode_Cand_expr</v>
       </c>
@@ -5513,7 +5071,7 @@
         <f>AD1&amp;"_"&amp;AE2</f>
         <v>ICDOTopographyCodeShort_Ref_expr</v>
       </c>
-      <c r="AF3" s="15" t="str">
+      <c r="AF3" s="6" t="str">
         <f>AD1&amp;"_"&amp;AF2</f>
         <v>ICDOTopographyCodeShort_Conn</v>
       </c>
@@ -5521,7 +5079,7 @@
         <f>AD1&amp;"_"&amp;AG2</f>
         <v>ICDOTopographyCodeShort_Cand_f</v>
       </c>
-      <c r="AH3" s="15" t="str">
+      <c r="AH3" s="6" t="str">
         <f>AD1&amp;"_"&amp;AH2</f>
         <v>ICDOTopographyCodeShort_Cand_expr</v>
       </c>
@@ -5537,7 +5095,7 @@
         <f>AJ1&amp;"_"&amp;AK2</f>
         <v>LocalizationSide_Ref_expr</v>
       </c>
-      <c r="AL3" s="15" t="str">
+      <c r="AL3" s="6" t="str">
         <f>AJ1&amp;"_"&amp;AL2</f>
         <v>LocalizationSide_Conn</v>
       </c>
@@ -5545,7 +5103,7 @@
         <f>AJ1&amp;"_"&amp;AM2</f>
         <v>LocalizationSide_Cand_f</v>
       </c>
-      <c r="AN3" s="15" t="str">
+      <c r="AN3" s="6" t="str">
         <f>AJ1&amp;"_"&amp;AN2</f>
         <v>LocalizationSide_Cand_expr</v>
       </c>
@@ -5561,7 +5119,7 @@
         <f>AP1&amp;"_"&amp;AQ2</f>
         <v>ICDOMorphologyCode_Ref_expr</v>
       </c>
-      <c r="AR3" s="15" t="str">
+      <c r="AR3" s="6" t="str">
         <f>AP1&amp;"_"&amp;AR2</f>
         <v>ICDOMorphologyCode_Conn</v>
       </c>
@@ -5569,7 +5127,7 @@
         <f>AP1&amp;"_"&amp;AS2</f>
         <v>ICDOMorphologyCode_Cand_f</v>
       </c>
-      <c r="AT3" s="15" t="str">
+      <c r="AT3" s="6" t="str">
         <f>AP1&amp;"_"&amp;AT2</f>
         <v>ICDOMorphologyCode_Cand_expr</v>
       </c>
@@ -5585,7 +5143,7 @@
         <f>AV1&amp;"_"&amp;AW2</f>
         <v>ICDOMorphologyCodeShort_Ref_expr</v>
       </c>
-      <c r="AX3" s="15" t="str">
+      <c r="AX3" s="6" t="str">
         <f>AV1&amp;"_"&amp;AX2</f>
         <v>ICDOMorphologyCodeShort_Conn</v>
       </c>
@@ -5593,7 +5151,7 @@
         <f>AV1&amp;"_"&amp;AY2</f>
         <v>ICDOMorphologyCodeShort_Cand_f</v>
       </c>
-      <c r="AZ3" s="15" t="str">
+      <c r="AZ3" s="6" t="str">
         <f>AV1&amp;"_"&amp;AZ2</f>
         <v>ICDOMorphologyCodeShort_Cand_expr</v>
       </c>
@@ -5609,7 +5167,7 @@
         <f>BB1&amp;"_"&amp;BC2</f>
         <v>Grading_Ref_expr</v>
       </c>
-      <c r="BD3" s="15" t="str">
+      <c r="BD3" s="6" t="str">
         <f>BB1&amp;"_"&amp;BD2</f>
         <v>Grading_Conn</v>
       </c>
@@ -5617,7 +5175,7 @@
         <f>BB1&amp;"_"&amp;BE2</f>
         <v>Grading_Cand_f</v>
       </c>
-      <c r="BF3" s="15" t="str">
+      <c r="BF3" s="6" t="str">
         <f>BB1&amp;"_"&amp;BF2</f>
         <v>Grading_Cand_expr</v>
       </c>
@@ -5654,35 +5212,35 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="16" t="str">
+      <c r="H4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Z4" s="16" t="str">
+      <c r="Z4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
       <c r="AC4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AL4" s="16" t="str">
+      <c r="AL4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
       <c r="AO4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AR4" s="16" t="str">
+      <c r="AR4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
       <c r="AU4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="BD4" s="16" t="str">
+      <c r="BD4" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5703,7 +5261,7 @@
       <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -5723,7 +5281,7 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="N6" s="16" t="str">
+      <c r="N6" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5741,7 +5299,7 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="T7" s="16" t="str">
+      <c r="T7" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5759,7 +5317,7 @@
       <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="Z8" s="16" t="str">
+      <c r="Z8" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5777,7 +5335,7 @@
       <c r="E9" s="1">
         <v>4</v>
       </c>
-      <c r="AF9" s="16" t="str">
+      <c r="AF9" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5799,7 +5357,7 @@
       <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="16" t="str">
+      <c r="H10" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5821,11 +5379,11 @@
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="H11" s="16" t="str">
+      <c r="H11" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="N11" s="16" t="str">
+      <c r="N11" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5847,11 +5405,11 @@
       <c r="E12" s="1">
         <v>3</v>
       </c>
-      <c r="N12" s="16" t="str">
+      <c r="N12" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="T12" s="16" t="str">
+      <c r="T12" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5873,7 +5431,7 @@
       <c r="E13" s="1">
         <v>4</v>
       </c>
-      <c r="T13" s="16" t="str">
+      <c r="T13" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -5895,7 +5453,7 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="Z14" s="16" t="str">
+      <c r="Z14" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5917,11 +5475,11 @@
       <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="Z15" s="16" t="str">
+      <c r="Z15" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="AF15" s="16" t="str">
+      <c r="AF15" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -5943,7 +5501,7 @@
       <c r="E16" s="1">
         <v>3</v>
       </c>
-      <c r="AF16" s="16" t="str">
+      <c r="AF16" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -5962,7 +5520,7 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="AL17" s="16" t="s">
+      <c r="AL17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5983,10 +5541,10 @@
       <c r="AK18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AL18" s="16" t="s">
+      <c r="AL18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN18" s="16" t="s">
+      <c r="AN18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6007,10 +5565,10 @@
       <c r="AK19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AL19" s="16" t="s">
+      <c r="AL19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN19" s="16" t="s">
+      <c r="AN19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -6031,10 +5589,10 @@
       <c r="AK20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AL20" s="16" t="s">
+      <c r="AL20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN20" s="16" t="s">
+      <c r="AN20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6055,10 +5613,10 @@
       <c r="AK21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AL21" s="16" t="s">
+      <c r="AL21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN21" s="16" t="s">
+      <c r="AN21" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6076,7 +5634,7 @@
       <c r="E22" s="1">
         <v>6</v>
       </c>
-      <c r="AL22" s="16" t="str">
+      <c r="AL22" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -6095,7 +5653,7 @@
       <c r="E23" s="1">
         <v>1</v>
       </c>
-      <c r="AR23" s="16" t="str">
+      <c r="AR23" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -6107,18 +5665,18 @@
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="13" t="str">
+      <c r="C24" s="10" t="str">
         <f>"'Same entity'"</f>
         <v>'Same entity'</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="AR24" s="16" t="str">
+      <c r="AR24" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="AX24" s="16" t="str">
+      <c r="AX24" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -6137,7 +5695,7 @@
       <c r="E25" s="1">
         <v>3</v>
       </c>
-      <c r="AX25" s="16" t="str">
+      <c r="AX25" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -6156,7 +5714,7 @@
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="BD26" s="16" t="str">
+      <c r="BD26" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
@@ -6175,7 +5733,7 @@
       <c r="E27" s="1">
         <v>2</v>
       </c>
-      <c r="BD27" s="16" t="str">
+      <c r="BD27" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
@@ -6198,10 +5756,10 @@
         <f>"== 'Unknown'"</f>
         <v>== 'Unknown'</v>
       </c>
-      <c r="AL28" s="16" t="s">
+      <c r="AL28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN28" s="16" t="str">
+      <c r="AN28" s="1" t="str">
         <f>"%in% c('Left', 'Right', 'Midline', 'Bilateral', 'Inapplicable')"</f>
         <v>%in% c('Left', 'Right', 'Midline', 'Bilateral', 'Inapplicable')</v>
       </c>
@@ -6219,19 +5777,19 @@
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="H29" s="16" t="str">
+      <c r="H29" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="Z29" s="16" t="str">
+      <c r="Z29" s="1" t="str">
         <f>"=="</f>
         <v>==</v>
       </c>
-      <c r="AR29" s="16" t="str">
+      <c r="AR29" s="1" t="str">
         <f>"!="</f>
         <v>!=</v>
       </c>
-      <c r="AX29" s="17"/>
+      <c r="AX29" s="10"/>
     </row>
     <row r="30" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -6250,10 +5808,10 @@
         <f>"== 'Low grade'"</f>
         <v>== 'Low grade'</v>
       </c>
-      <c r="BD30" s="16" t="s">
+      <c r="BD30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="BF30" s="16" t="str">
+      <c r="BF30" s="1" t="str">
         <f>"== 'High grade'"</f>
         <v>== 'High grade'</v>
       </c>
@@ -6276,10 +5834,10 @@
         <f>"%in% c('Left', 'Right', 'Midline', 'Bilateral')"</f>
         <v>%in% c('Left', 'Right', 'Midline', 'Bilateral')</v>
       </c>
-      <c r="AL31" s="16" t="s">
+      <c r="AL31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN31" s="16" t="str">
+      <c r="AN31" s="1" t="str">
         <f>"== 'Unknown'"</f>
         <v>== 'Unknown'</v>
       </c>
@@ -6302,10 +5860,10 @@
         <f>"== 'Inapplicable'"</f>
         <v>== 'Inapplicable'</v>
       </c>
-      <c r="AL32" s="16" t="s">
+      <c r="AL32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AN32" s="16" t="str">
+      <c r="AN32" s="1" t="str">
         <f>"%in% c('Left', 'Right', 'Midline', 'Bilateral')"</f>
         <v>%in% c('Left', 'Right', 'Midline', 'Bilateral')</v>
       </c>

</xml_diff>

<commit_message>
Improved performance of ClassifyDiagnosis functions
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/RuleSets.xlsx
+++ b/Development/Data/MetaData/RuleSets.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BFFAA4-1A8F-4634-8D80-A3E136F3F074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9637B7F5-CEE0-4E7C-AD83-9B52EF51BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="DiagnosisAssociation" sheetId="16" r:id="rId1"/>
-    <sheet name="DiagnosisRedundancies" sheetId="20" r:id="rId2"/>
+    <sheet name="DiagnosisRedundancy" sheetId="20" r:id="rId2"/>
     <sheet name="ExcludeRawData" sheetId="18" r:id="rId3"/>
     <sheet name="TempBackup" sheetId="19" r:id="rId4"/>
   </sheets>
@@ -1826,10 +1826,10 @@
   <dimension ref="A1:BD30"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3089,7 +3089,7 @@
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implemented hash table lookup in transformation
</commit_message>
<xml_diff>
--- a/Development/Data/MetaData/RuleSets.xlsx
+++ b/Development/Data/MetaData/RuleSets.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsCCPhos\Development\Data\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F61EEDA-DE1D-453E-A0D8-C77A157B809F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979DAD14-3F14-4B89-86CC-21E5529C8B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="RawDataExclusion" sheetId="18" r:id="rId1"/>
     <sheet name="RawDataTransformation" sheetId="21" r:id="rId2"/>
-    <sheet name="DiagnosisRedundancy" sheetId="20" r:id="rId3"/>
-    <sheet name="DiagnosisAssociation" sheetId="16" r:id="rId4"/>
-    <sheet name="TempBackup" sheetId="19" r:id="rId5"/>
+    <sheet name="RawDataTransformationBACKUP" sheetId="22" r:id="rId3"/>
+    <sheet name="DiagnosisRedundancy" sheetId="20" r:id="rId4"/>
+    <sheet name="DiagnosisAssociation" sheetId="16" r:id="rId5"/>
+    <sheet name="TempBackup" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="141">
   <si>
     <t>Grading</t>
   </si>
@@ -428,6 +429,39 @@
   </si>
   <si>
     <t>rp</t>
+  </si>
+  <si>
+    <t>is(dcis)</t>
+  </si>
+  <si>
+    <t>is(lcis)</t>
+  </si>
+  <si>
+    <t>1(sm)</t>
+  </si>
+  <si>
+    <t>1(sm1)</t>
+  </si>
+  <si>
+    <t>1(sm2)</t>
+  </si>
+  <si>
+    <t>1(sm3)</t>
+  </si>
+  <si>
+    <t>1(sn3)</t>
+  </si>
+  <si>
+    <t>x(sn)</t>
+  </si>
+  <si>
+    <t>LookupValue</t>
+  </si>
+  <si>
+    <t>NewValue</t>
+  </si>
+  <si>
+    <t>HashTable</t>
   </si>
 </sst>
 </file>
@@ -2521,7 +2555,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2554,10 +2588,10 @@
         <v>64</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>63</v>
@@ -2651,10 +2685,10 @@
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>89</v>
@@ -2779,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>85</v>
@@ -2805,7 +2839,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>86</v>
@@ -2828,10 +2862,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>89</v>
@@ -2891,10 +2925,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>80</v>
@@ -2917,10 +2951,10 @@
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>81</v>
@@ -2940,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>78</v>
@@ -2986,10 +3020,10 @@
         <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>84</v>
@@ -3012,10 +3046,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>84</v>
@@ -3035,10 +3069,10 @@
         <v>14</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>84</v>
@@ -3058,10 +3092,10 @@
         <v>15</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>84</v>
@@ -3081,10 +3115,10 @@
         <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>84</v>
@@ -3161,10 +3195,10 @@
         <v>20</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>91</v>
@@ -3184,7 +3218,7 @@
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>92</v>
@@ -3406,7 +3440,7 @@
         <v>33</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>106</v>
@@ -3429,7 +3463,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>108</v>
@@ -3452,7 +3486,7 @@
         <v>35</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>110</v>
@@ -3475,7 +3509,7 @@
         <v>35</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>127</v>
@@ -3498,7 +3532,7 @@
         <v>35</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>128</v>
@@ -3521,7 +3555,7 @@
         <v>35</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>129</v>
@@ -3578,7 +3612,7 @@
         <v>38</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>106</v>
@@ -3601,7 +3635,7 @@
         <v>39</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>108</v>
@@ -3624,7 +3658,7 @@
         <v>40</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>110</v>
@@ -3647,7 +3681,7 @@
         <v>38</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>127</v>
@@ -3670,7 +3704,7 @@
         <v>39</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>128</v>
@@ -3693,7 +3727,7 @@
         <v>40</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>129</v>
@@ -3750,7 +3784,7 @@
         <v>43</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>106</v>
@@ -3773,7 +3807,7 @@
         <v>44</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>108</v>
@@ -3796,7 +3830,7 @@
         <v>45</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>110</v>
@@ -3819,7 +3853,7 @@
         <v>43</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>127</v>
@@ -3842,7 +3876,7 @@
         <v>44</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>128</v>
@@ -3865,7 +3899,7 @@
         <v>45</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>129</v>
@@ -3881,6 +3915,1373 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE4BB71C-D47E-498B-867C-D9D9123699DA}">
+  <dimension ref="A1:H64"/>
+  <sheetViews>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="94.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="1" customWidth="1"/>
+    <col min="8" max="8" width="63.6640625" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="16.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="1">
+        <v>12</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="1">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="1">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="1">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="1">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="1">
+        <v>18</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="1">
+        <v>19</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="1">
+        <v>20</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="1">
+        <v>21</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="1">
+        <v>22</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="1">
+        <v>23</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="1">
+        <v>24</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="1">
+        <v>26</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="1">
+        <v>27</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="1">
+        <v>28</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="1">
+        <v>29</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="1">
+        <v>30</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="1">
+        <v>31</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="1">
+        <v>32</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="1">
+        <v>33</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D44" s="1">
+        <v>34</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="1">
+        <v>35</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D46" s="1">
+        <v>35</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" s="1">
+        <v>35</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D48" s="1">
+        <v>35</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="1">
+        <v>36</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="1">
+        <v>37</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="1">
+        <v>38</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="1">
+        <v>39</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="1">
+        <v>40</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="1">
+        <v>38</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" s="1">
+        <v>39</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="1">
+        <v>40</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="1">
+        <v>41</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="1">
+        <v>42</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="1">
+        <v>43</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D60" s="1">
+        <v>44</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="1">
+        <v>45</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D62" s="1">
+        <v>43</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D63" s="1">
+        <v>44</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D64" s="1">
+        <v>45</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF34485D-2E08-41A5-8940-99532983F125}">
   <dimension ref="A1:AT29"/>
   <sheetViews>
@@ -4982,7 +6383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDC58E-646F-4995-A1CB-0FC9545134E1}">
   <dimension ref="A1:BD30"/>
   <sheetViews>
@@ -4990,7 +6391,7 @@
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6242,15 +7643,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE52532-6DED-4B4A-9AA4-16253C1E26AB}">
-  <dimension ref="A1:BL32"/>
+  <dimension ref="A1:BM64"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="BD48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="BM1" sqref="BM1:BM66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6291,10 +7692,11 @@
     <col min="59" max="59" width="11.33203125" style="9" customWidth="1"/>
     <col min="60" max="60" width="20.109375" style="1" customWidth="1"/>
     <col min="61" max="64" width="27.5546875" style="1" customWidth="1"/>
-    <col min="65" max="16384" width="16.33203125" style="1"/>
+    <col min="65" max="65" width="17.6640625" style="1" customWidth="1"/>
+    <col min="66" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6377,8 +7779,11 @@
       <c r="BJ1" s="2"/>
       <c r="BK1" s="2"/>
       <c r="BL1" s="2"/>
-    </row>
-    <row r="2" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM1" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6552,7 +7957,7 @@
       <c r="BK2" s="2"/>
       <c r="BL2" s="2"/>
     </row>
-    <row r="3" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -6800,7 +8205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -6846,7 +8251,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="5" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -6869,7 +8274,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -6886,8 +8291,11 @@
         <f>"=="</f>
         <v>==</v>
       </c>
-    </row>
-    <row r="7" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM6" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -6905,7 +8313,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -6923,7 +8331,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="9" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -6941,7 +8349,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="10" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -6963,7 +8371,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="11" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -6989,7 +8397,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="12" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -7015,7 +8423,7 @@
         <v>==</v>
       </c>
     </row>
-    <row r="13" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -7036,8 +8444,11 @@
         <f>"!="</f>
         <v>!=</v>
       </c>
-    </row>
-    <row r="14" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM13" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -7058,8 +8469,11 @@
         <f>"=="</f>
         <v>==</v>
       </c>
-    </row>
-    <row r="15" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM14" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -7084,8 +8498,11 @@
         <f>"=="</f>
         <v>==</v>
       </c>
-    </row>
-    <row r="16" spans="1:64" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM15" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -7107,7 +8524,7 @@
         <v>!=</v>
       </c>
     </row>
-    <row r="17" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -7125,7 +8542,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -7148,8 +8565,11 @@
       <c r="AN18" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
@@ -7172,8 +8592,11 @@
       <c r="AN19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM19" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
@@ -7196,8 +8619,11 @@
       <c r="AN20" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -7220,8 +8646,11 @@
       <c r="AN21" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -7239,8 +8668,11 @@
         <f>"!="</f>
         <v>!=</v>
       </c>
-    </row>
-    <row r="23" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -7258,8 +8690,11 @@
         <f>"=="</f>
         <v>==</v>
       </c>
-    </row>
-    <row r="24" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM23" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -7281,8 +8716,11 @@
         <f>"=="</f>
         <v>==</v>
       </c>
-    </row>
-    <row r="25" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM24" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -7300,8 +8738,11 @@
         <f>"!="</f>
         <v>!=</v>
       </c>
-    </row>
-    <row r="26" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM25" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -7319,8 +8760,11 @@
         <f>"=="</f>
         <v>==</v>
       </c>
-    </row>
-    <row r="27" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM26" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -7339,7 +8783,7 @@
         <v>!=</v>
       </c>
     </row>
-    <row r="28" spans="1:58" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:65" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -7365,7 +8809,7 @@
         <v>%in% c('Left', 'Right', 'Midline', 'Bilateral', 'Inapplicable')</v>
       </c>
     </row>
-    <row r="29" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -7391,8 +8835,11 @@
         <v>!=</v>
       </c>
       <c r="AX29" s="10"/>
-    </row>
-    <row r="30" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM29" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -7416,8 +8863,11 @@
         <f>"== 'High grade'"</f>
         <v>== 'High grade'</v>
       </c>
-    </row>
-    <row r="31" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM30" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -7442,8 +8892,11 @@
         <f>"== 'Unknown'"</f>
         <v>== 'Unknown'</v>
       </c>
-    </row>
-    <row r="32" spans="1:58" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM31" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -7467,6 +8920,101 @@
       <c r="AN32" s="1" t="str">
         <f>"%in% c('Left', 'Right', 'Midline', 'Bilateral')"</f>
         <v>%in% c('Left', 'Right', 'Midline', 'Bilateral')</v>
+      </c>
+    </row>
+    <row r="34" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM34" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM43" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM44" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM45" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM46" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM47" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM48" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM51" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM52" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM53" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM54" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM55" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM56" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM59" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="60" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM60" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM61" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM62" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM63" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="65:65" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="BM64" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>